<commit_message>
remove-products-expiration-date.py ready for verification
</commit_message>
<xml_diff>
--- a/Barcodes sold.xlsx
+++ b/Barcodes sold.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lander Wuyts\IT\Sys Eng Projectweek\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EC5E3C5-98B4-4997-BED6-1860BF9A7068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49859590-2BDC-4911-92E5-F5C3CA37449A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5239CB96-FA84-43C4-98A1-2144099ABCCF}"/>
   </bookViews>
@@ -90,9 +90,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -410,16 +412,17 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="14.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -427,24 +430,24 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>40833666</v>
+      <c r="A2" s="3">
+        <v>7610700949085</v>
       </c>
       <c r="B2">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>65165465</v>
+      <c r="A3" s="3">
+        <v>5414150631147</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>65416564</v>
+      <c r="A4" s="3">
+        <v>8719200099616</v>
       </c>
       <c r="B4">
         <v>1</v>

</xml_diff>

<commit_message>
changed add code to read all cells instead of last one
</commit_message>
<xml_diff>
--- a/Barcodes sold.xlsx
+++ b/Barcodes sold.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lander Wuyts\IT\Sys Eng Projectweek\Python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49859590-2BDC-4911-92E5-F5C3CA37449A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6373AA04-7B03-48EB-8F20-7029ECE1DADC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5239CB96-FA84-43C4-98A1-2144099ABCCF}"/>
   </bookViews>
@@ -409,10 +409,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8315AB79-82FD-4F9F-8156-629013D4B21E}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -442,15 +442,47 @@
         <v>5414150631147</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
-        <v>8719200099616</v>
+        <v>7610700949085</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>3502110008091</v>
+      </c>
+      <c r="B5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>5410013110002</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>5411028070480</v>
+      </c>
+      <c r="B7">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>5411188115472</v>
+      </c>
+      <c r="B8">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>